<commit_message>
correction orthographes + ajout test
</commit_message>
<xml_diff>
--- a/Tableau Test TODO IT Now.xlsx
+++ b/Tableau Test TODO IT Now.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="103">
   <si>
     <t>TYPE</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>intégration</t>
+  </si>
+  <si>
+    <t>Afficher le timesheet d'un utilisateur préalablement connecté pour test la fonctionnalité de lecture de données en BDD et voir s'il est possible d'obtenir la timesheet d'un utilisateur grâce à son JWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renvoie la timesheet de l'utilisateur proprietaire du JWT envoyé au serveur </t>
+  </si>
+  <si>
+    <t>Réussite: Affiche la timesheet de l'utilisateur sur la page web / Echec: renvoie un message d'erreur (404 ou 500 en fonction du probleme) ou renvoie un objet vide ou renvoie une timesheet ne correspondant pas au bon utilisateur</t>
   </si>
   <si>
     <t>tester la lecture d'informations apres la connexion d'un utilisateurs via requete POST (envoyé via des formulaires ou directement lorsque l'utilisateur se présente sur une page en fonction de son role</t>
@@ -459,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -532,6 +541,9 @@
     </xf>
     <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1013,7 +1025,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="25" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1106,22 +1118,22 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="9">
+        <v>44956.0</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="9">
-        <v>44956.0</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>10</v>
@@ -1129,7 +1141,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>56</v>
@@ -1152,7 +1164,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>59</v>
@@ -1175,7 +1187,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>62</v>
@@ -1198,7 +1210,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>65</v>
@@ -1221,22 +1233,22 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="9">
+        <v>44956.0</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="9">
-        <v>44957.0</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>10</v>
@@ -1244,13 +1256,13 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="9">
-        <v>44958.0</v>
+        <v>44957.0</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>73</v>
@@ -1267,22 +1279,22 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C23" s="9">
-        <v>44959.0</v>
+        <v>44958.0</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>10</v>
@@ -1290,22 +1302,22 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="9">
-        <v>44960.0</v>
+        <v>44959.0</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>10</v>
@@ -1313,22 +1325,22 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" s="9">
-        <v>44961.0</v>
+        <v>44960.0</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>10</v>
@@ -1336,22 +1348,22 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="9">
-        <v>44962.0</v>
+        <v>44961.0</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>10</v>
@@ -1359,16 +1371,16 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" s="9">
-        <v>44963.0</v>
+        <v>44962.0</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>10</v>
@@ -1382,13 +1394,13 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C28" s="9">
-        <v>44964.0</v>
+        <v>44963.0</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>87</v>
@@ -1397,7 +1409,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>10</v>
@@ -1405,22 +1417,22 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="9">
+        <v>44964.0</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="C29" s="9">
-        <v>44965.0</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>10</v>
@@ -1428,22 +1440,22 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C30" s="9">
-        <v>44966.0</v>
+        <v>44965.0</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>10</v>
@@ -1451,13 +1463,13 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C31" s="9">
-        <v>44967.0</v>
+        <v>44966.0</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>94</v>
@@ -1474,24 +1486,47 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="9">
+        <v>44967.0</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="9">
+      <c r="E32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="9">
         <v>44969.0</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="G32" s="10" t="s">
+      <c r="D33" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>